<commit_message>
Misurati con ohmmetro, valutare anche linearità
</commit_message>
<xml_diff>
--- a/circuiti20240307/20240307circuiti.xlsx
+++ b/circuiti20240307/20240307circuiti.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="voltmetro" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="amperometro" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="VRI" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="test resistenze" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>R(MOHM)</t>
   </si>
@@ -37,13 +38,29 @@
   <si>
     <t xml:space="preserve">NOTA: da cella 15 il voltmetro misura solo 2 ciffre dopo la virgola, valutare errore</t>
   </si>
+  <si>
+    <t xml:space="preserve">R attesa</t>
+  </si>
+  <si>
+    <t>exponent</t>
+  </si>
+  <si>
+    <t>Rmisurata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTA: aggiungere 0.3 ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(misurati con ohmmetro)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -73,10 +90,18 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1165,4 +1190,471 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="26.8515625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5.4000000000000004</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.2999999999999998</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.4000000000000004</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10.300000000000001</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.996</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="4">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.992</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="4">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4.0090000000000003</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="4">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5.0060000000000002</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="4">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6.0039999999999996</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="4">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7.0099999999999998</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="4">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>8.0099999999999998</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="4">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="4">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="4">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5">
+        <v>100.09999999999999</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="4">
+        <v>200</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5">
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="4">
+        <v>300</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="5">
+        <v>303.5</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="4">
+        <v>400</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="4">
+        <v>500</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="4">
+        <v>600</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="6">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="6">
+        <v>0.80000000000000004</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="6">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>1.012</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="4">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>2.0219999999999998</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="4">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>2.9910000000000001</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="4">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>4.0350000000000001</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="4">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>5.0449999999999999</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="4">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>6.0549999999999997</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="4">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>7.0199999999999996</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="4">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>8.0299999999999994</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="4">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>9.0399999999999991</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="4">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
soglia diodo raccolti dati
</commit_message>
<xml_diff>
--- a/circuiti20240307/20240307circuiti.xlsx
+++ b/circuiti20240307/20240307circuiti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="voltmetro" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="test resistenze" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="resistenze composite parallelo" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="resistenze composite serie" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="soglia diodo" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>R(MOHM)</t>
   </si>
@@ -73,6 +74,9 @@
   <si>
     <t xml:space="preserve">NOTA: usata config 2</t>
   </si>
+  <si>
+    <t xml:space="preserve">NOTA: attorno ai 0.7-0.8 i valori sono sulla soglia</t>
+  </si>
 </sst>
 </file>
 
@@ -122,7 +126,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1691,14 +1695,14 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="12.7109375"/>
     <col customWidth="1" min="2" max="2" width="13.00390625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
@@ -1737,7 +1741,6 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4"/>
       <c r="C4" s="2">
         <v>1.5029999999999999</v>
       </c>
@@ -1840,13 +1843,13 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
@@ -1970,6 +1973,197 @@
       </c>
       <c r="D14" s="1">
         <v>29.920000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="46.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>0.059999999999999998</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.0050000000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.0050000000000000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>0.249</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.025000000000000001</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.59199999999999997</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="B10" s="2">
+        <v>11.890000000000001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>40.270000000000003</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="B12" s="1">
+        <v>123.63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="B13" s="1">
+        <v>234.84999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="B14" s="1">
+        <v>375.42000000000002</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="B15" s="1">
+        <v>574.25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>0.745</v>
+      </c>
+      <c r="B16" s="1">
+        <v>732.10000000000002</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="B17" s="1">
+        <v>937.70000000000005</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="B18" s="7">
+        <v>36863</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="B19" s="7">
+        <v>53710</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="B20" s="7">
+        <v>71790</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <v>0.999</v>
+      </c>
+      <c r="B21" s="7">
+        <v>87254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fatti conti soglia dal basso (prima di ordinarli
</commit_message>
<xml_diff>
--- a/circuiti20240307/20240307circuiti.xlsx
+++ b/circuiti20240307/20240307circuiti.xlsx
@@ -12,7 +12,7 @@
     <sheet name="test resistenze" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="resistenze composite parallelo" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="resistenze composite serie" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="soglia diodo" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="soglia diodo crescenti" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -1986,7 +1986,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2166,6 +2166,158 @@
         <v>87254</v>
       </c>
     </row>
+    <row r="22" ht="14.25">
+      <c r="A22">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="B22">
+        <v>326.60000000000002</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="B23">
+        <v>360.30000000000001</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="B24">
+        <v>396.69999999999999</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="B25">
+        <v>432.60000000000002</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="B26">
+        <v>507.30000000000001</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="B27">
+        <v>545.20000000000005</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="B28">
+        <v>585.89999999999998</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="B29">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="B30">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="B31">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="B32">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="B33">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="B34">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="B35">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="B36">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="B37">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="B38">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="B39">
+        <v>47450</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="B40">
+        <v>57120</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
dati diodo al contrario
</commit_message>
<xml_diff>
--- a/circuiti20240307/20240307circuiti.xlsx
+++ b/circuiti20240307/20240307circuiti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="voltmetro" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="resistenze composite parallelo" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="resistenze composite serie" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="soglia diodo crescenti" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="soglia diodo discendente" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>R(MOHM)</t>
   </si>
@@ -76,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">NOTA: attorno ai 0.7-0.8 i valori sono sulla soglia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTA: presi in ordine decrescente</t>
   </si>
 </sst>
 </file>
@@ -2322,4 +2326,232 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="B2">
+        <v>83950</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="B3" s="7">
+        <v>80623</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="B4" s="7">
+        <v>65630</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="B5" s="7">
+        <v>57443</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="B6" s="7">
+        <v>51095</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="B7" s="7">
+        <v>47950</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43340</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="B9" s="7">
+        <v>33040</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="B10" s="7">
+        <v>24780</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="B11" s="7">
+        <v>21925</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>0.78000000000000003</v>
+      </c>
+      <c r="B12" s="7">
+        <v>18460</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>0.77000000000000002</v>
+      </c>
+      <c r="B13" s="7">
+        <v>16165</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>0.76000000000000001</v>
+      </c>
+      <c r="B14" s="7">
+        <v>14020</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="B15" s="7">
+        <v>11045</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>0.72999999999999998</v>
+      </c>
+      <c r="B16" s="7">
+        <v>8509</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="B17" s="7">
+        <v>6312</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="B18" s="7">
+        <v>3580</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="B20" s="7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="B21" s="7">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="B22" s="7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="B23" s="1">
+        <v>31.379999999999999</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8.1300000000000008</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.77000000000000002</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
diodo datas is good
</commit_message>
<xml_diff>
--- a/circuiti20240307/20240307circuiti.xlsx
+++ b/circuiti20240307/20240307circuiti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="voltmetro" sheetId="1" state="visible" r:id="rId1"/>
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
@@ -130,8 +130,6 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1992,7 +1990,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2189,10 +2187,10 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="8">
+      <c r="A24" s="2">
         <v>0.745</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>732.10000000000002</v>
       </c>
     </row>
@@ -2221,10 +2219,10 @@
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="8">
+      <c r="A28" s="2">
         <v>0.79700000000000004</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="7">
         <v>937</v>
       </c>
     </row>
@@ -2285,10 +2283,10 @@
       </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="8">
+      <c r="A36" s="2">
         <v>0.89900000000000002</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="7">
         <v>53710</v>
       </c>
     </row>
@@ -2301,18 +2299,18 @@
       </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="8">
+      <c r="A38" s="2">
         <v>0.95399999999999996</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="7">
         <v>71790</v>
       </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="8">
+      <c r="A39" s="2">
         <v>0.999</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="7">
         <v>87254</v>
       </c>
     </row>
@@ -2335,7 +2333,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>